<commit_message>
[INITIAL COMMIT] - Filter datatable within number of X days, and also added handling for rows with empty birthday.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan.ely.garchitorena\Documents\UiPath\GetUpcomingBirthdays\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\CET_BirthdayGreetings\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BC91F1-3125-425D-B317-B1CA92F60347}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FE1945-CFDB-4EA9-B727-A3CD95FE5072}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -127,18 +127,9 @@
     <t>BirthdayList_Path</t>
   </si>
   <si>
-    <t>Filepath of the excel spreadsheet</t>
-  </si>
-  <si>
-    <t>C:\Users\%UserProfile%\Documents\UiPath\Birthday Greeting Postcard\C-ET Birthday List.xlsx</t>
-  </si>
-  <si>
     <t>BirthdayList_Range</t>
   </si>
   <si>
-    <t>""</t>
-  </si>
-  <si>
     <t>BirthdayList_SheetName</t>
   </si>
   <si>
@@ -148,7 +139,28 @@
     <t>Sheet name of list of birthdays in the excel spreadsheet</t>
   </si>
   <si>
-    <t>Range to be read in the birthday list excel spreadsheet</t>
+    <t>Filepath of the excel spreadsheet. Where UserProfile is the name of the logged user</t>
+  </si>
+  <si>
+    <t>C:\Users\{{UserProfile}}\Documents\UiPath\Birthday Greeting Postcard\C-ET Birthday List.xlsx</t>
+  </si>
+  <si>
+    <t>Range to be read in the birthday list excel spreadsheet. Keep the value emptied to read all cells in the spreadsheet</t>
+  </si>
+  <si>
+    <t>UpcomingBirthdayRange</t>
+  </si>
+  <si>
+    <t>Value in number of days to determine upcoming birthdays within range (DateToday - X days)</t>
+  </si>
+  <si>
+    <t>Exception_BirthdayListNotExist</t>
+  </si>
+  <si>
+    <t>Exception message if the list of birthday excel file does not exist</t>
+  </si>
+  <si>
+    <t>Birthday master list does not exist</t>
   </si>
 </sst>
 </file>
@@ -526,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -600,37 +612,44 @@
       <c r="A6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" t="s">
-        <v>34</v>
+      <c r="B6" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1630,7 +1649,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -1754,7 +1775,17 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
[INITIAL COMMIT] - Generate excel file for each upcoming birthday celebrant's team members and additional team (Management)
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\CET_BirthdayGreetings\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FE1945-CFDB-4EA9-B727-A3CD95FE5072}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7C653D-BA19-4B8C-AA81-1BDB733F35D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="2040" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -148,9 +148,6 @@
     <t>Range to be read in the birthday list excel spreadsheet. Keep the value emptied to read all cells in the spreadsheet</t>
   </si>
   <si>
-    <t>UpcomingBirthdayRange</t>
-  </si>
-  <si>
     <t>Value in number of days to determine upcoming birthdays within range (DateToday - X days)</t>
   </si>
   <si>
@@ -161,6 +158,42 @@
   </si>
   <si>
     <t>Birthday master list does not exist</t>
+  </si>
+  <si>
+    <t>UpcomingBirthday_Range</t>
+  </si>
+  <si>
+    <t>UpcomingBirthday_OutputFolder</t>
+  </si>
+  <si>
+    <t>C:\Users\{{UserProfile}}\Documents\UiPath\Birthday Greeting Postcard\Upcoming birthdays</t>
+  </si>
+  <si>
+    <t>Filepath of the upcoming birthday celebrant's team mates</t>
+  </si>
+  <si>
+    <t>UpcomingBirthday_IncludeTeam</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>Included team when consolidating the celebrant's team members. Only accepts 1 team. Write "n/a" if you do not wish to include other team.</t>
+  </si>
+  <si>
+    <t>BirthdayList_Index_EID</t>
+  </si>
+  <si>
+    <t>BirthdayList_Index_Birthday</t>
+  </si>
+  <si>
+    <t>BirthdayList_Index_Team</t>
+  </si>
+  <si>
+    <t>Column index of "Birthday" in BirthdayList datatable</t>
+  </si>
+  <si>
+    <t>Column index of "Team" in BirthdayList datatable</t>
   </si>
 </sst>
 </file>
@@ -536,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -641,21 +674,71 @@
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
         <v>40</v>
       </c>
-      <c r="B10">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>41</v>
-      </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -1638,6 +1721,10 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
+    <row r="1002" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1649,7 +1736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -1777,13 +1864,13 @@
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
         <v>42</v>
-      </c>
-      <c r="B12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
[INITIAL COMMIT] - Send email to celebrant's team members plus management - Values for the Email Subject and Body are not yet finalized
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\CET_BirthdayGreetings\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7C653D-BA19-4B8C-AA81-1BDB733F35D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E79A67C-310A-48C3-8BA9-B098E04E5B6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="2040" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3765" yWindow="3765" windowWidth="23895" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -194,6 +194,21 @@
   </si>
   <si>
     <t>Column index of "Team" in BirthdayList datatable</t>
+  </si>
+  <si>
+    <t>Email_Subject</t>
+  </si>
+  <si>
+    <t>Email_Body</t>
+  </si>
+  <si>
+    <t>Email subject to be sent to the team members and management</t>
+  </si>
+  <si>
+    <t>Email body to be sent to the team members and management</t>
+  </si>
+  <si>
+    <t>Testing - Automated Birthday Greeting Postcard</t>
   </si>
 </sst>
 </file>
@@ -572,7 +587,7 @@
   <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -739,22 +754,42 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
[CODE OPTIMIZE] - Added condition for special resources in filtering datatable for the sending of email. If EID is identified as a special resource, then get all resources. Else, filter only the celebrant's team and management.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\CET_BirthdayGreetings\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E79A67C-310A-48C3-8BA9-B098E04E5B6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39670EBC-89AD-488F-92DC-B269FF8D36CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="3765" windowWidth="23895" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -209,6 +209,18 @@
   </si>
   <si>
     <t>Testing - Automated Birthday Greeting Postcard</t>
+  </si>
+  <si>
+    <t>Column index of "EID" in BirthdayList datatable</t>
+  </si>
+  <si>
+    <t>lorelie.a.pangan;sarah.c.c.layug;johnell.m.hernandez</t>
+  </si>
+  <si>
+    <t>UpcomingBirthday_MandatoryEIDGetAll</t>
+  </si>
+  <si>
+    <t>If one of the upcoming bday celebrant is here, all resources will be sent an email to ask for birthday greetings</t>
   </si>
 </sst>
 </file>
@@ -584,11 +596,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1002"/>
+  <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -706,7 +716,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -754,30 +764,40 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" t="s">
-        <v>58</v>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" t="s">
+        <v>64</v>
       </c>
     </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" t="s">
         <v>60</v>
       </c>
       <c r="C19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1760,6 +1780,7 @@
     <row r="1000" ht="14.25" customHeight="1"/>
     <row r="1001" ht="14.25" customHeight="1"/>
     <row r="1002" ht="14.25" customHeight="1"/>
+    <row r="1003" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[CODE OPTIMIZE] - Updated team name of management to "Management I"  - Added bday celebrant's name (Resource Name) in the subject in all capital letters  - Added hyperlink in the email body to be redirected to sharepoint
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\CET_BirthdayGreetings\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39670EBC-89AD-488F-92DC-B269FF8D36CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F32DC74-5292-437E-B572-096EE7755D98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3570" yWindow="1905" windowWidth="23895" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
   <si>
     <t>Name</t>
   </si>
@@ -175,9 +175,6 @@
     <t>UpcomingBirthday_IncludeTeam</t>
   </si>
   <si>
-    <t>Management</t>
-  </si>
-  <si>
     <t>Included team when consolidating the celebrant's team members. Only accepts 1 team. Write "n/a" if you do not wish to include other team.</t>
   </si>
   <si>
@@ -202,25 +199,37 @@
     <t>Email_Body</t>
   </si>
   <si>
-    <t>Email subject to be sent to the team members and management</t>
-  </si>
-  <si>
     <t>Email body to be sent to the team members and management</t>
   </si>
   <si>
-    <t>Testing - Automated Birthday Greeting Postcard</t>
-  </si>
-  <si>
     <t>Column index of "EID" in BirthdayList datatable</t>
   </si>
   <si>
+    <t>UpcomingBirthday_MandatoryEIDGetAll</t>
+  </si>
+  <si>
+    <t>If one of the upcoming bday celebrant is here, all resources will be sent an email to ask for birthday greetings</t>
+  </si>
+  <si>
+    <t>Management I</t>
+  </si>
+  <si>
+    <t>Testing - upcoming birthday for: {0}</t>
+  </si>
+  <si>
+    <t>Email subject to be sent to the team members and management. Where 0 is the value for the celebrant's name.</t>
+  </si>
+  <si>
+    <t>BirthdayList_Index_ResourceName</t>
+  </si>
+  <si>
+    <t>Column index of "Resource Name" in BirthdayList datatable</t>
+  </si>
+  <si>
     <t>lorelie.a.pangan;sarah.c.c.layug;johnell.m.hernandez</t>
   </si>
   <si>
-    <t>UpcomingBirthday_MandatoryEIDGetAll</t>
-  </si>
-  <si>
-    <t>If one of the upcoming bday celebrant is here, all resources will be sent an email to ask for birthday greetings</t>
+    <t>Testing - Please send your birthday greetings &lt;a href="https://ts.accenture.com/sites/Chevron_PDC/CET/Lists/CET%20Birthday%20Greetings/AllItems.aspx"&gt;here&lt;/href&gt;</t>
   </si>
 </sst>
 </file>
@@ -596,9 +605,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1003"/>
+  <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -699,13 +710,13 @@
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -713,92 +724,102 @@
         <v>51</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13">
         <v>7</v>
       </c>
-      <c r="C12" t="s">
-        <v>55</v>
+      <c r="C13" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" t="s">
         <v>60</v>
       </c>
-      <c r="C19" t="s">
-        <v>58</v>
-      </c>
     </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
         <v>57</v>
       </c>
-      <c r="B20" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" t="s">
-        <v>59</v>
-      </c>
     </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1781,6 +1802,7 @@
     <row r="1001" ht="14.25" customHeight="1"/>
     <row r="1002" ht="14.25" customHeight="1"/>
     <row r="1003" ht="14.25" customHeight="1"/>
+    <row r="1004" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[CODE OPTIMIZE] - Save sent emails for upcoming birthday celebrants to skip them on the next run
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\CET_BirthdayGreetings\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F32DC74-5292-437E-B572-096EE7755D98}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43071B69-D580-4EEF-A0E9-FA53B4C13ECC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3570" yWindow="1905" windowWidth="23895" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -608,7 +608,7 @@
   <dimension ref="A1:Z1004"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
[CODE OPTIMIZE] - Consolidation of upcoming birthdays to send an email to specific resources 1 by 1 1. Separation of specific resource(s) from other team for the email recipients 2. Adding of the specific resource(s) to another group of data for the sending of email to each specific resource 3. Additional condition and handling to remove the specific resource(s) if it is for his/her birthday message 4. Composition of email body for the consolidated upcoming birthdays 5. Sending of separate email for the specific resource(s)
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\CET_BirthdayGreetings\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43071B69-D580-4EEF-A0E9-FA53B4C13ECC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACB044F-45F8-43BD-B1FD-578091BEBA4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4125" yWindow="1695" windowWidth="23895" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="77">
   <si>
     <t>Name</t>
   </si>
@@ -214,9 +214,6 @@
     <t>Management I</t>
   </si>
   <si>
-    <t>Testing - upcoming birthday for: {0}</t>
-  </si>
-  <si>
     <t>Email subject to be sent to the team members and management. Where 0 is the value for the celebrant's name.</t>
   </si>
   <si>
@@ -229,14 +226,102 @@
     <t>lorelie.a.pangan;sarah.c.c.layug;johnell.m.hernandez</t>
   </si>
   <si>
-    <t>Testing - Please send your birthday greetings &lt;a href="https://ts.accenture.com/sites/Chevron_PDC/CET/Lists/CET%20Birthday%20Greetings/AllItems.aspx"&gt;here&lt;/href&gt;</t>
+    <t>ConsolidateEmailEachResource</t>
+  </si>
+  <si>
+    <t>A separate email will be sent to each of these resources (EID) separated by semi-colon (;) for the consolidation of upcoming birthdays</t>
+  </si>
+  <si>
+    <t>EmailConsolidated_Subject</t>
+  </si>
+  <si>
+    <t>EmailConsolidated_Body</t>
+  </si>
+  <si>
+    <t>[C-ET] Upcoming Birthdays: {0}</t>
+  </si>
+  <si>
+    <t>[C-ET] Upcoming Birthdays</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Email body to be sent to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ConsolidateEmailResource</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>. Where 0 is the value for the name of celebrants.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Email subject to be sent to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ConsolidateEmailResource</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+  </si>
+  <si>
+    <t>Hi All,&lt;br&gt;
+&lt;br&gt;
+Good Day! We've identified that one (or more) of your colleagues will celebrate his/her birthday soon. &lt;br&gt;
+Make their day extra special by sending them your greetings via the &lt;b&gt;C-ET Birthday Postcard&lt;/b&gt;! &lt;br&gt;
+&lt;br&gt;
+Use the links below to log your greetings:&lt;br&gt;
+&lt;br&gt;
+{0}
+&lt;br&gt;
+(This is an automated email. Do not forward)</t>
+  </si>
+  <si>
+    <t>Hi All,&lt;br&gt;
+&lt;br&gt;
+Good day! We've identified that one (or more) of your colleagues will celebrate his/her birthday soon. &lt;br&gt;
+Make their day extra special by sending them your greetings via the &lt;b&gt;C-ET Birthday Postcard&lt;/b&gt;! &lt;br&gt;
+&lt;br&gt;
+Use this &lt;a href="https://ts.accenture.com/sites/Chevron_PDC/CET/Lists/CET%20Birthday%20Greetings/AllItems.aspx"&gt;link&lt;/a&gt;  to log you greetings. &lt;br&gt;
+&lt;br&gt;
+(This is an automated email. Do not forward)</t>
+  </si>
+  <si>
+    <t>johnell.m.hernandez</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -247,6 +332,7 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
@@ -255,6 +341,13 @@
       <charset val="128"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -605,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1004"/>
+  <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -710,13 +803,13 @@
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -791,7 +884,7 @@
         <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
         <v>60</v>
@@ -803,28 +896,58 @@
         <v>55</v>
       </c>
       <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" t="s">
         <v>62</v>
-      </c>
-      <c r="C20" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
         <v>56</v>
       </c>
-      <c r="B21" t="s">
-        <v>67</v>
+      <c r="B21" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="C21" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1803,6 +1926,8 @@
     <row r="1002" ht="14.25" customHeight="1"/>
     <row r="1003" ht="14.25" customHeight="1"/>
     <row r="1004" ht="14.25" customHeight="1"/>
+    <row r="1005" ht="14.25" customHeight="1"/>
+    <row r="1006" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[CODE OPTIMIZE] - Use nickname in the subject instead of full resource name
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\CET_BirthdayGreetings\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACB044F-45F8-43BD-B1FD-578091BEBA4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17434A8-9585-4834-B053-51EFD4CD9FCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4125" yWindow="1695" windowWidth="23895" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -315,6 +315,12 @@
   </si>
   <si>
     <t>johnell.m.hernandez</t>
+  </si>
+  <si>
+    <t>BirthdayList_Index_Nickname</t>
+  </si>
+  <si>
+    <t>Column index of "Nickname" in BirthdayList datatable</t>
   </si>
 </sst>
 </file>
@@ -698,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1006"/>
+  <dimension ref="A1:Z1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -814,141 +820,151 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
         <v>52</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>7</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15">
-        <v>14</v>
-      </c>
-      <c r="C15" t="s">
-        <v>40</v>
-      </c>
-    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
         <v>59</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>65</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" t="s">
-        <v>62</v>
-      </c>
-    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A23" t="s">
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
         <v>66</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>76</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A25" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1928,6 +1944,7 @@
     <row r="1004" ht="14.25" customHeight="1"/>
     <row r="1005" ht="14.25" customHeight="1"/>
     <row r="1006" ht="14.25" customHeight="1"/>
+    <row r="1007" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
undo changes in email subject
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\CET_BirthdayGreetings\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17434A8-9585-4834-B053-51EFD4CD9FCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB4A54A-E10C-411A-B023-E464DC077B52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4125" yWindow="1695" windowWidth="23895" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="77">
   <si>
     <t>Name</t>
   </si>
@@ -315,12 +315,6 @@
   </si>
   <si>
     <t>johnell.m.hernandez</t>
-  </si>
-  <si>
-    <t>BirthdayList_Index_Nickname</t>
-  </si>
-  <si>
-    <t>Column index of "Nickname" in BirthdayList datatable</t>
   </si>
 </sst>
 </file>
@@ -704,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1007"/>
+  <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -820,151 +814,141 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>54</v>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16">
-        <v>14</v>
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" t="s">
-        <v>60</v>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" t="s">
-        <v>70</v>
+        <v>56</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A22" t="s">
-        <v>56</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" t="s">
-        <v>57</v>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A24" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24" t="s">
-        <v>76</v>
-      </c>
-      <c r="C24" t="s">
-        <v>67</v>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A27" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1944,7 +1928,6 @@
     <row r="1004" ht="14.25" customHeight="1"/>
     <row r="1005" ht="14.25" customHeight="1"/>
     <row r="1006" ht="14.25" customHeight="1"/>
-    <row r="1007" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[INITIAL COMMIT[ - Creation of sharepoint item to each of the specific resources.  - Capturing of sharepoint URL of the created item.  - Sharing of sharepoint URL to the specific resources in the email.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\CET_BirthdayGreetings\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB4A54A-E10C-411A-B023-E464DC077B52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9F6389-1794-407E-B1DB-25857BBFDC01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4125" yWindow="1695" windowWidth="23895" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="82">
   <si>
     <t>Name</t>
   </si>
@@ -314,7 +314,22 @@
 (This is an automated email. Do not forward)</t>
   </si>
   <si>
-    <t>johnell.m.hernandez</t>
+    <t>Sharepoint_BirthdayGreetings</t>
+  </si>
+  <si>
+    <t>https://ts.accenture.com/sites/Chevron_PDC/CET/Lists/CET%20Birthday%20Greetings/AllItems.aspx</t>
+  </si>
+  <si>
+    <t>TimeoutShort</t>
+  </si>
+  <si>
+    <t>Timeout for a short duration</t>
+  </si>
+  <si>
+    <t>johnell.m.hernandez;lorelie.a.pangan</t>
+  </si>
+  <si>
+    <t>URL to be opened during initialize state for the home page of Birthday Greetings.</t>
   </si>
 </sst>
 </file>
@@ -374,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -384,6 +399,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -919,7 +935,7 @@
         <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
         <v>67</v>
@@ -949,7 +965,17 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" t="s">
+        <v>81</v>
+      </c>
+    </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1940,7 +1966,7 @@
   <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2077,7 +2103,17 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14">
+        <v>5000</v>
+      </c>
+      <c r="C14" t="s">
+        <v>79</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>

</xml_diff>